<commit_message>
Added association relationships to UML diagram
</commit_message>
<xml_diff>
--- a/UML Diagram.xlsx
+++ b/UML Diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucd-my.sharepoint.com/personal/michael_davitt_ucdconnect_ie/Documents/Documents/Projects/Secret_Santa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="262" documentId="8_{972F4980-7E40-49BA-A048-13EA752BEBFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B22EBC37-002C-4AFB-BEAF-7DE544295BC7}"/>
+  <xr:revisionPtr revIDLastSave="302" documentId="8_{972F4980-7E40-49BA-A048-13EA752BEBFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C9EF79D-D2B5-4983-B6EB-9CE819632842}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A00B6DC3-DED0-4EAA-AA01-7BF2577D2AED}"/>
   </bookViews>
@@ -103,16 +103,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>117365</xdr:rowOff>
+      <xdr:rowOff>69740</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -127,7 +127,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2381250" y="688865"/>
+          <a:off x="971550" y="641240"/>
           <a:ext cx="2047875" cy="3387834"/>
           <a:chOff x="4362450" y="974615"/>
           <a:chExt cx="2047875" cy="1966414"/>
@@ -368,16 +368,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -392,7 +392,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2381250" y="4400550"/>
+          <a:off x="1000125" y="4543425"/>
           <a:ext cx="2047875" cy="2076450"/>
           <a:chOff x="4362450" y="974615"/>
           <a:chExt cx="2047875" cy="2076450"/>
@@ -572,14 +572,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -596,7 +596,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9067800" y="714375"/>
+          <a:off x="13849350" y="714375"/>
           <a:ext cx="2047875" cy="2371725"/>
           <a:chOff x="4362450" y="974615"/>
           <a:chExt cx="2047875" cy="2371725"/>
@@ -785,16 +785,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>82660</xdr:rowOff>
+      <xdr:rowOff>101710</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -809,7 +809,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12163425" y="714375"/>
+          <a:off x="6696075" y="733425"/>
           <a:ext cx="2047875" cy="1844785"/>
           <a:chOff x="4362450" y="974615"/>
           <a:chExt cx="2047875" cy="1844785"/>
@@ -984,16 +984,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>357188</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>166688</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>357188</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>195263</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1010,9 +1010,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="3405188" y="4076699"/>
-          <a:ext cx="0" cy="323851"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1995488" y="4029074"/>
+          <a:ext cx="28575" cy="514351"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1040,16 +1040,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -1064,7 +1064,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5800725" y="714375"/>
+          <a:off x="6696075" y="3086100"/>
           <a:ext cx="2047875" cy="2952750"/>
           <a:chOff x="5800725" y="714375"/>
           <a:chExt cx="2047875" cy="2952750"/>
@@ -1305,6 +1305,522 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>126089</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>141343</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F7D3B7F-9647-40AB-9C3C-C366A16952FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="28" idx="1"/>
+          <a:endCxn id="3" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3019425" y="1650089"/>
+          <a:ext cx="3676650" cy="15254"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>126089</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8D1D33A-592F-4FE5-9D26-057ACF5C83EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="3"/>
+          <a:endCxn id="15" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3019425" y="781050"/>
+          <a:ext cx="828675" cy="869039"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Rectangle 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCCEF714-7902-49D1-8C90-AF69CEE7C0C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3848100" y="247650"/>
+          <a:ext cx="1962150" cy="1066800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>Many-to-many relationship:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100" baseline="0"/>
+            <a:t> Participants can have many gifts in their wishlist, and gifts can be present in many participant's wishlists</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>117531</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>141343</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Straight Connector 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FA64B44-4C4D-40B0-8A2D-5717866591B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="20" idx="1"/>
+          <a:endCxn id="28" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8743950" y="1641531"/>
+          <a:ext cx="5105400" cy="23812"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="Rectangle 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FCDF04E-24C4-46BA-AA4F-9639DE8F0982}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10334625" y="238125"/>
+          <a:ext cx="1962150" cy="1066800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>Many-to-many relationship:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100" baseline="0"/>
+            <a:t> A market can have many gifts, and gifts can be sold in many markets</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>141343</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Straight Connector 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19A80940-8611-496C-803D-D78CDA4835A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="28" idx="3"/>
+          <a:endCxn id="38" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8743950" y="771525"/>
+          <a:ext cx="1590675" cy="893818"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Straight Connector 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7F872A1-AFB9-420D-8127-41AB730A5484}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="50" idx="0"/>
+          <a:endCxn id="4" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3019425" y="3109912"/>
+          <a:ext cx="1743075" cy="738188"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>154098</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="Straight Connector 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74A52335-B097-427F-9AF5-D9E8FB633A23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="23" idx="1"/>
+          <a:endCxn id="4" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3019425" y="3109912"/>
+          <a:ext cx="3676650" cy="282686"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Rectangle 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12DA4F28-D17B-4BB6-8B83-E6665DE80B61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3781425" y="3848100"/>
+          <a:ext cx="1962150" cy="1066800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100"/>
+            <a:t>One-to-many</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1100" baseline="0"/>
+            <a:t> relationship: A group can have many participants, but a participant can belong to at most one group</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1610,7 +2126,7 @@
   <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>